<commit_message>
Umarbeitungen an der Datenbank. Tests laufen derzeit deswegen nicht.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Neuanlage Mitarbeiter.xlsx
+++ b/src/main/Mitarbeiterdaten/Neuanlage Mitarbeiter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689C5C61-5959-4B70-9E54-13D62B8FCF7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F49559-6451-49DC-BE78-0ED88E5E6210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="107">
   <si>
     <t>11 111 111 111</t>
   </si>
@@ -157,9 +157,6 @@
     <t>Zuschuss privater Zusatzbeitrag</t>
   </si>
   <si>
-    <t>Zuschuss private Pflegeversicheurng</t>
-  </si>
-  <si>
     <t>Zuschuss private Krankenversicherung</t>
   </si>
   <si>
@@ -346,10 +343,10 @@
     <t>KKH</t>
   </si>
   <si>
-    <t>Zusatzbeitrag Krankenversicherung in Prozent</t>
-  </si>
-  <si>
     <t>Kaufmaennische Krankenkasse</t>
+  </si>
+  <si>
+    <t>Zuschuss private Pflegeversicherung</t>
   </si>
 </sst>
 </file>
@@ -483,7 +480,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -501,18 +498,30 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -935,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -960,7 +969,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D2" s="10"/>
     </row>
@@ -969,7 +978,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -985,7 +994,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" s="10"/>
     </row>
@@ -1109,7 +1118,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19" s="10"/>
     </row>
@@ -1118,7 +1127,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D20" s="10"/>
     </row>
@@ -1136,7 +1145,7 @@
         <v>33</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D22" s="10"/>
     </row>
@@ -1145,7 +1154,7 @@
         <v>34</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D23" s="10"/>
     </row>
@@ -1153,7 +1162,7 @@
       <c r="A24" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="21">
         <v>1</v>
       </c>
       <c r="D24" s="10"/>
@@ -1162,7 +1171,7 @@
       <c r="A25" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="22">
         <v>35</v>
       </c>
       <c r="D25" s="10"/>
@@ -1171,26 +1180,26 @@
       <c r="A26" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>54</v>
+      <c r="B26" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="D26" s="10"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>55</v>
+        <v>67</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="D27" s="10"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="D28" s="10"/>
     </row>
@@ -1198,8 +1207,8 @@
       <c r="A29" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>65</v>
+      <c r="B29" s="23" t="s">
+        <v>64</v>
       </c>
       <c r="D29" s="10"/>
     </row>
@@ -1207,8 +1216,8 @@
       <c r="A30" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>66</v>
+      <c r="B30" s="23" t="s">
+        <v>65</v>
       </c>
       <c r="D30" s="10"/>
     </row>
@@ -1216,182 +1225,182 @@
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>70</v>
+      <c r="B31" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="D32" s="10"/>
     </row>
     <row r="33" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>64</v>
+        <v>45</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>63</v>
       </c>
       <c r="D33" s="10"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>104</v>
+        <v>74</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>75</v>
       </c>
       <c r="D34" s="10"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>76</v>
+        <v>41</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>103</v>
       </c>
       <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" s="9">
+        <v>71</v>
+      </c>
+      <c r="B36" s="26">
         <v>3523.76</v>
       </c>
       <c r="D36" s="10"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" s="9">
+        <v>72</v>
+      </c>
+      <c r="B37" s="26">
         <v>1254.28</v>
       </c>
       <c r="D37" s="10"/>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" s="9">
+        <v>73</v>
+      </c>
+      <c r="B38" s="26">
         <v>2568.75</v>
       </c>
       <c r="D38" s="10"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>57</v>
+        <v>99</v>
+      </c>
+      <c r="B39" s="27" t="s">
+        <v>56</v>
       </c>
       <c r="D39" s="10"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="B40" s="28"/>
       <c r="D40" s="10"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B41" s="2"/>
+      <c r="B41" s="28"/>
       <c r="D41" s="10"/>
     </row>
     <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="2"/>
+        <v>106</v>
+      </c>
+      <c r="B42" s="28"/>
       <c r="D42" s="10"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>64</v>
+        <v>79</v>
+      </c>
+      <c r="B43" s="29" t="s">
+        <v>63</v>
       </c>
       <c r="D43" s="10"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B44" s="5">
+        <v>92</v>
+      </c>
+      <c r="B44" s="30">
         <v>7.3</v>
       </c>
       <c r="D44" s="10"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B45" s="5">
+        <v>93</v>
+      </c>
+      <c r="B45" s="30">
         <v>7.3</v>
       </c>
       <c r="D45" s="10"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B46" s="5">
+        <v>94</v>
+      </c>
+      <c r="B46" s="30">
         <v>72000</v>
       </c>
       <c r="D46" s="10"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B47" s="5">
+        <v>95</v>
+      </c>
+      <c r="B47" s="30">
         <v>68000</v>
       </c>
       <c r="D47" s="10"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>107</v>
+        <v>48</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>105</v>
       </c>
       <c r="D48" s="10"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>105</v>
+        <v>47</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="D49" s="10"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B50" s="5">
-        <v>1.5</v>
+      <c r="A50" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" s="22">
+        <v>2</v>
       </c>
       <c r="D50" s="10"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B51" s="8">
-        <v>2</v>
+        <v>96</v>
+      </c>
+      <c r="B51" s="22">
+        <v>1</v>
       </c>
       <c r="D51" s="10"/>
     </row>
@@ -1399,8 +1408,8 @@
       <c r="A52" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B52" s="8">
-        <v>1</v>
+      <c r="B52" s="22">
+        <v>35000</v>
       </c>
       <c r="D52" s="10"/>
     </row>
@@ -1408,44 +1417,44 @@
       <c r="A53" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B53" s="8">
-        <v>35000</v>
+      <c r="B53" s="22">
+        <v>38000</v>
       </c>
       <c r="D53" s="10"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B54" s="8">
-        <v>38000</v>
+        <v>44</v>
+      </c>
+      <c r="B54" s="31" t="s">
+        <v>63</v>
       </c>
       <c r="D54" s="10"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>64</v>
+    <row r="55" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B55" s="32">
+        <v>1.2</v>
       </c>
       <c r="D55" s="10"/>
     </row>
-    <row r="56" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="B56" s="18">
-        <v>1.2</v>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="D56" s="10"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>64</v>
+        <v>86</v>
+      </c>
+      <c r="B57" s="33">
+        <v>3.7</v>
       </c>
       <c r="D57" s="10"/>
     </row>
@@ -1453,7 +1462,7 @@
       <c r="A58" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B58" s="22">
+      <c r="B58" s="33">
         <v>3.7</v>
       </c>
       <c r="D58" s="10"/>
@@ -1462,94 +1471,85 @@
       <c r="A59" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B59" s="22">
-        <v>3.7</v>
+      <c r="B59" s="33">
+        <v>64123</v>
       </c>
       <c r="D59" s="10"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B60" s="22">
-        <v>64123</v>
+      <c r="B60" s="34">
+        <v>68543</v>
       </c>
       <c r="D60" s="10"/>
     </row>
-    <row r="61" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B61" s="23">
-        <v>68543</v>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B61" s="35" t="s">
+        <v>63</v>
       </c>
       <c r="D61" s="10"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="19" t="s">
+      <c r="A62" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B62" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="D62" s="11"/>
+      <c r="B62" s="36">
+        <v>10.3</v>
+      </c>
+      <c r="D62" s="10"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B63" s="25">
+      <c r="B63" s="36">
         <v>10.3</v>
       </c>
-      <c r="D63" s="11"/>
+      <c r="D63" s="10"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B64" s="25">
-        <v>10.3</v>
-      </c>
-      <c r="D64" s="11"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="7" t="s">
+      <c r="B64" s="36">
+        <v>78563.45</v>
+      </c>
+      <c r="D64" s="10"/>
+    </row>
+    <row r="65" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B65" s="25">
-        <v>78563.45</v>
-      </c>
-      <c r="D65" s="11"/>
-    </row>
-    <row r="66" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B66" s="26">
+      <c r="B65" s="37">
         <v>81253</v>
       </c>
+      <c r="D65" s="10"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B66" s="38"/>
       <c r="D66" s="11"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B67" s="27"/>
+        <v>90</v>
+      </c>
+      <c r="B67" s="39"/>
       <c r="D67" s="11"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="5" t="s">
+    <row r="68" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B68" s="27"/>
+      <c r="B68" s="40"/>
       <c r="D68" s="11"/>
-    </row>
-    <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="B69" s="28"/>
-      <c r="D69" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1589,13 +1589,13 @@
           <x14:formula1>
             <xm:f>Tabelle2!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B28 B39 B43 B57 B62 B67 B33 B55</xm:sqref>
+          <xm:sqref>B28 B39 B43 B56 B61 B66 B33 B54</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BC540D61-4588-479B-B62B-BA6755FB2963}">
           <x14:formula1>
             <xm:f>Tabelle2!$I$2:$I$102</xm:f>
           </x14:formula1>
-          <xm:sqref>B51</xm:sqref>
+          <xm:sqref>B50</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1630,24 +1630,24 @@
         <v>40</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1655,16 +1655,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -1672,10 +1672,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -1686,7 +1686,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1697,7 +1697,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -1708,7 +1708,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E7">
         <v>6</v>

</xml_diff>

<commit_message>
SQL-Code angepasst. Tests wuerden derzeit nicht laufen.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Neuanlage Mitarbeiter.xlsx
+++ b/src/main/Mitarbeiterdaten/Neuanlage Mitarbeiter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F49559-6451-49DC-BE78-0ED88E5E6210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EA835C-A795-4BBD-A933-756A11D51891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -241,15 +241,6 @@
     <t>BSR</t>
   </si>
   <si>
-    <t>Grundgehalt</t>
-  </si>
-  <si>
-    <t>Weihnachtsgeld</t>
-  </si>
-  <si>
-    <t>Urlaubgeld</t>
-  </si>
-  <si>
     <t>Gewerkschaft</t>
   </si>
   <si>
@@ -347,6 +338,15 @@
   </si>
   <si>
     <t>Zuschuss private Pflegeversicherung</t>
+  </si>
+  <si>
+    <t>Grundgehalt aussertariflich</t>
+  </si>
+  <si>
+    <t>Weihnachtsgeld aussertariflich</t>
+  </si>
+  <si>
+    <t>Urlaubgeld aussertariflich</t>
   </si>
 </sst>
 </file>
@@ -946,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -969,7 +969,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D2" s="10"/>
     </row>
@@ -978,7 +978,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -994,7 +994,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D5" s="10"/>
     </row>
@@ -1250,10 +1250,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D34" s="10"/>
     </row>
@@ -1262,13 +1262,13 @@
         <v>41</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="B36" s="26">
         <v>3523.76</v>
@@ -1277,7 +1277,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="B37" s="26">
         <v>1254.28</v>
@@ -1286,7 +1286,7 @@
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="B38" s="26">
         <v>2568.75</v>
@@ -1295,7 +1295,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B39" s="27" t="s">
         <v>56</v>
@@ -1318,14 +1318,14 @@
     </row>
     <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B42" s="28"/>
       <c r="D42" s="10"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B43" s="29" t="s">
         <v>63</v>
@@ -1334,7 +1334,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B44" s="30">
         <v>7.3</v>
@@ -1343,7 +1343,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B45" s="30">
         <v>7.3</v>
@@ -1352,7 +1352,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B46" s="30">
         <v>72000</v>
@@ -1361,7 +1361,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B47" s="30">
         <v>68000</v>
@@ -1373,7 +1373,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D48" s="10"/>
     </row>
@@ -1382,7 +1382,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D49" s="10"/>
     </row>
@@ -1397,7 +1397,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B51" s="22">
         <v>1</v>
@@ -1406,7 +1406,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B52" s="22">
         <v>35000</v>
@@ -1415,7 +1415,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B53" s="22">
         <v>38000</v>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="55" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="17" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B55" s="32">
         <v>1.2</v>
@@ -1442,7 +1442,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>63</v>
@@ -1451,7 +1451,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B57" s="33">
         <v>3.7</v>
@@ -1460,7 +1460,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B58" s="33">
         <v>3.7</v>
@@ -1469,7 +1469,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B59" s="33">
         <v>64123</v>
@@ -1478,7 +1478,7 @@
     </row>
     <row r="60" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B60" s="34">
         <v>68543</v>
@@ -1487,7 +1487,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B61" s="35" t="s">
         <v>63</v>
@@ -1496,7 +1496,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B62" s="36">
         <v>10.3</v>
@@ -1505,7 +1505,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B63" s="36">
         <v>10.3</v>
@@ -1514,7 +1514,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B64" s="36">
         <v>78563.45</v>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="65" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B65" s="37">
         <v>81253</v>
@@ -1539,14 +1539,14 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B67" s="39"/>
       <c r="D67" s="11"/>
     </row>
     <row r="68" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="20" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B68" s="40"/>
       <c r="D68" s="11"/>
@@ -1630,7 +1630,7 @@
         <v>40</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>66</v>
@@ -1708,7 +1708,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E7">
         <v>6</v>

</xml_diff>